<commit_message>
Solicitud grafica cuaderno de estudio
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion05/SolicitudesGraficas/SolicitudGrafica_MA_07_05_CO_REC10.xlsx
+++ b/fuentes/contenidos/grado07/guion05/SolicitudesGraficas/SolicitudGrafica_MA_07_05_CO_REC10.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\---Adriana\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion05\SolicitudesGraficas_Edicion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\---Adriana\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion05\SolicitudesGraficas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="hX79YNGfHMUCcosWMoH0GQuhNo2gkebFrfW3do2TOcvwqaujU9m0uwOL5UkRtWEspAy/ISD2JB8+jf057W9mVA==" workbookSaltValue="uRz/CDpmZ5ecKheoN1C0Jw==" workbookSpinCount="100000" lockStructure="1"/>
@@ -593,9 +593,6 @@
     <t>Ilustración</t>
   </si>
   <si>
-    <t>MA_09_02_REC10</t>
-  </si>
-  <si>
     <t>Los números racionales</t>
   </si>
   <si>
@@ -706,6 +703,9 @@
     <t>La imagen fue tomada de shutterstock: 178307564
 Incluir el globo de pensamiento con la división.
 4a ficha del menú 3</t>
+  </si>
+  <si>
+    <t>MA_07_05_REC10</t>
   </si>
 </sst>
 </file>
@@ -1660,6 +1660,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1716,12 +1722,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -3069,7 +3069,7 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3178,7 +3178,7 @@
         <v>54</v>
       </c>
       <c r="C4" s="81" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D4" s="82"/>
       <c r="E4" s="5"/>
@@ -3209,10 +3209,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="101" t="s">
-        <v>190</v>
-      </c>
-      <c r="D5" s="102"/>
+      <c r="C5" s="83" t="s">
+        <v>189</v>
+      </c>
+      <c r="D5" s="84"/>
       <c r="E5" s="5"/>
       <c r="F5" s="37" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -3267,7 +3267,7 @@
         <v>40</v>
       </c>
       <c r="C7" s="68" t="s">
-        <v>188</v>
+        <v>215</v>
       </c>
       <c r="D7" s="23" t="s">
         <v>39</v>
@@ -3363,7 +3363,7 @@
         <v>IMG01</v>
       </c>
       <c r="B10" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C10" s="20" t="str">
         <f t="shared" ref="C10:C41" si="0">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
@@ -3377,7 +3377,7 @@
       </c>
       <c r="F10" s="13" t="str">
         <f t="shared" ref="F10" ca="1" si="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>MA_09_02_REC10_IMG01.jpg</v>
+        <v>MA_07_05_REC10_IMG01.jpg</v>
       </c>
       <c r="G10" s="13" t="str">
         <f ca="1">IF($F10&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E10,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3392,7 +3392,7 @@
         <v/>
       </c>
       <c r="J10" s="63" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K10" s="64"/>
       <c r="O10" s="2" t="str">
@@ -3413,14 +3413,14 @@
         <v>Recurso F6</v>
       </c>
       <c r="D11" s="63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E11" s="63" t="s">
         <v>150</v>
       </c>
       <c r="F11" s="13" t="str">
         <f t="shared" ref="F11:F74" ca="1" si="4">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
-        <v>MA_09_02_REC10_IMG02.jpg</v>
+        <v>MA_07_05_REC10_IMG02.jpg</v>
       </c>
       <c r="G11" s="13" t="str">
         <f ca="1">IF($F11&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E11,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3435,7 +3435,7 @@
         <v/>
       </c>
       <c r="J11" s="64" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K11" s="64"/>
       <c r="O11" s="2" t="str">
@@ -3456,14 +3456,14 @@
         <v>Recurso F6</v>
       </c>
       <c r="D12" s="63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E12" s="63" t="s">
         <v>150</v>
       </c>
       <c r="F12" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG03.jpg</v>
+        <v>MA_07_05_REC10_IMG03.jpg</v>
       </c>
       <c r="G12" s="13" t="str">
         <f ca="1">IF($F12&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E12,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3478,7 +3478,7 @@
         <v/>
       </c>
       <c r="J12" s="64" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="K12" s="64"/>
       <c r="O12" s="2" t="str">
@@ -3492,7 +3492,7 @@
         <v>IMG04</v>
       </c>
       <c r="B13" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C13" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3506,7 +3506,7 @@
       </c>
       <c r="F13" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG04n.jpg</v>
+        <v>MA_07_05_REC10_IMG04n.jpg</v>
       </c>
       <c r="G13" s="13" t="str">
         <f ca="1">IF($F13&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3514,17 +3514,17 @@
       </c>
       <c r="H13" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG04a.jpg</v>
+        <v>MA_07_05_REC10_IMG04a.jpg</v>
       </c>
       <c r="I13" s="13" t="str">
         <f ca="1">IF(OR($B13&lt;&gt;"",$J13&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E13,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J13" s="63" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="K13" s="64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O13" s="2" t="str">
         <f>'Definición técnica de imagenes'!A19</f>
@@ -3537,7 +3537,7 @@
         <v>IMG05</v>
       </c>
       <c r="B14" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C14" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3551,7 +3551,7 @@
       </c>
       <c r="F14" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG05n.jpg</v>
+        <v>MA_07_05_REC10_IMG05n.jpg</v>
       </c>
       <c r="G14" s="13" t="str">
         <f ca="1">IF($F14&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3559,17 +3559,17 @@
       </c>
       <c r="H14" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG05a.jpg</v>
+        <v>MA_07_05_REC10_IMG05a.jpg</v>
       </c>
       <c r="I14" s="13" t="str">
         <f ca="1">IF(OR($B14&lt;&gt;"",$J14&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E14,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J14" s="63" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="K14" s="64" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O14" s="2" t="str">
         <f>'Definición técnica de imagenes'!A22</f>
@@ -3582,7 +3582,7 @@
         <v>IMG06</v>
       </c>
       <c r="B15" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C15" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3596,7 +3596,7 @@
       </c>
       <c r="F15" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG06n.jpg</v>
+        <v>MA_07_05_REC10_IMG06n.jpg</v>
       </c>
       <c r="G15" s="13" t="str">
         <f ca="1">IF($F15&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3604,14 +3604,14 @@
       </c>
       <c r="H15" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG06a.jpg</v>
+        <v>MA_07_05_REC10_IMG06a.jpg</v>
       </c>
       <c r="I15" s="13" t="str">
         <f ca="1">IF(OR($B15&lt;&gt;"",$J15&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E15,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J15" s="63" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="K15" s="64"/>
       <c r="O15" s="2" t="str">
@@ -3625,7 +3625,7 @@
         <v>IMG07</v>
       </c>
       <c r="B16" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C16" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3639,7 +3639,7 @@
       </c>
       <c r="F16" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG07n.jpg</v>
+        <v>MA_07_05_REC10_IMG07n.jpg</v>
       </c>
       <c r="G16" s="13" t="str">
         <f ca="1">IF($F16&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3647,17 +3647,17 @@
       </c>
       <c r="H16" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG07a.jpg</v>
+        <v>MA_07_05_REC10_IMG07a.jpg</v>
       </c>
       <c r="I16" s="13" t="str">
         <f ca="1">IF(OR($B16&lt;&gt;"",$J16&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E16,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J16" s="63" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="K16" s="64" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O16" s="2" t="str">
         <f>'Definición técnica de imagenes'!A25</f>
@@ -3670,7 +3670,7 @@
         <v>IMG08</v>
       </c>
       <c r="B17" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C17" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3684,7 +3684,7 @@
       </c>
       <c r="F17" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG08n.jpg</v>
+        <v>MA_07_05_REC10_IMG08n.jpg</v>
       </c>
       <c r="G17" s="13" t="str">
         <f ca="1">IF($F17&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3692,17 +3692,17 @@
       </c>
       <c r="H17" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG08a.jpg</v>
+        <v>MA_07_05_REC10_IMG08a.jpg</v>
       </c>
       <c r="I17" s="13" t="str">
         <f ca="1">IF(OR($B17&lt;&gt;"",$J17&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E17,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J17" s="63" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="K17" s="64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O17" s="2" t="str">
         <f>'Definición técnica de imagenes'!A27</f>
@@ -3715,7 +3715,7 @@
         <v>IMG09</v>
       </c>
       <c r="B18" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C18" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3729,7 +3729,7 @@
       </c>
       <c r="F18" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG09n.jpg</v>
+        <v>MA_07_05_REC10_IMG09n.jpg</v>
       </c>
       <c r="G18" s="13" t="str">
         <f ca="1">IF($F18&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3737,17 +3737,17 @@
       </c>
       <c r="H18" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG09a.jpg</v>
+        <v>MA_07_05_REC10_IMG09a.jpg</v>
       </c>
       <c r="I18" s="13" t="str">
         <f ca="1">IF(OR($B18&lt;&gt;"",$J18&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E18,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J18" s="63" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="K18" s="64" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O18" s="2" t="str">
         <f>'Definición técnica de imagenes'!A30</f>
@@ -3767,14 +3767,14 @@
         <v>Recurso F6</v>
       </c>
       <c r="D19" s="63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E19" s="63" t="s">
         <v>155</v>
       </c>
       <c r="F19" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG10n.jpg</v>
+        <v>MA_07_05_REC10_IMG10n.jpg</v>
       </c>
       <c r="G19" s="13" t="str">
         <f ca="1">IF($F19&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3782,17 +3782,17 @@
       </c>
       <c r="H19" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG10a.jpg</v>
+        <v>MA_07_05_REC10_IMG10a.jpg</v>
       </c>
       <c r="I19" s="13" t="str">
         <f ca="1">IF(OR($B19&lt;&gt;"",$J19&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E19,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J19" s="63" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K19" s="64" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="O19" s="2" t="str">
         <f>'Definición técnica de imagenes'!A31</f>
@@ -3805,7 +3805,7 @@
         <v>IMG11</v>
       </c>
       <c r="B20" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C20" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3819,7 +3819,7 @@
       </c>
       <c r="F20" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG11n.jpg</v>
+        <v>MA_07_05_REC10_IMG11n.jpg</v>
       </c>
       <c r="G20" s="13" t="str">
         <f ca="1">IF($F20&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3827,17 +3827,17 @@
       </c>
       <c r="H20" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG11a.jpg</v>
+        <v>MA_07_05_REC10_IMG11a.jpg</v>
       </c>
       <c r="I20" s="13" t="str">
         <f ca="1">IF(OR($B20&lt;&gt;"",$J20&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E20,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J20" s="63" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K20" s="64" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="O20" s="2" t="str">
         <f>'Definición técnica de imagenes'!A32</f>
@@ -3850,7 +3850,7 @@
         <v>IMG12</v>
       </c>
       <c r="B21" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C21" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3864,7 +3864,7 @@
       </c>
       <c r="F21" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG12n.jpg</v>
+        <v>MA_07_05_REC10_IMG12n.jpg</v>
       </c>
       <c r="G21" s="13" t="str">
         <f ca="1">IF($F21&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3872,17 +3872,17 @@
       </c>
       <c r="H21" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG12a.jpg</v>
+        <v>MA_07_05_REC10_IMG12a.jpg</v>
       </c>
       <c r="I21" s="13" t="str">
         <f ca="1">IF(OR($B21&lt;&gt;"",$J21&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E21,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J21" s="63" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K21" s="64" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O21" s="2" t="str">
         <f>'Definición técnica de imagenes'!A33</f>
@@ -3895,7 +3895,7 @@
         <v>IMG13</v>
       </c>
       <c r="B22" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C22" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3909,7 +3909,7 @@
       </c>
       <c r="F22" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG13n.jpg</v>
+        <v>MA_07_05_REC10_IMG13n.jpg</v>
       </c>
       <c r="G22" s="13" t="str">
         <f ca="1">IF($F22&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E22,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3917,17 +3917,17 @@
       </c>
       <c r="H22" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG13a.jpg</v>
+        <v>MA_07_05_REC10_IMG13a.jpg</v>
       </c>
       <c r="I22" s="13" t="str">
         <f ca="1">IF(OR($B22&lt;&gt;"",$J22&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E22,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E22,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J22" s="63" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K22" s="64" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O22" s="2" t="str">
         <f>'Definición técnica de imagenes'!A34</f>
@@ -3947,14 +3947,14 @@
         <v>Recurso F6</v>
       </c>
       <c r="D23" s="63" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E23" s="63" t="s">
         <v>155</v>
       </c>
       <c r="F23" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG14n.jpg</v>
+        <v>MA_07_05_REC10_IMG14n.jpg</v>
       </c>
       <c r="G23" s="13" t="str">
         <f ca="1">IF($F23&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E23,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -3962,14 +3962,14 @@
       </c>
       <c r="H23" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG14a.jpg</v>
+        <v>MA_07_05_REC10_IMG14a.jpg</v>
       </c>
       <c r="I23" s="13" t="str">
         <f ca="1">IF(OR($B23&lt;&gt;"",$J23&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E23,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E23,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J23" s="63" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K23" s="64"/>
       <c r="O23" s="2" t="str">
@@ -3983,7 +3983,7 @@
         <v>IMG15</v>
       </c>
       <c r="B24" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C24" s="20" t="str">
         <f t="shared" si="0"/>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="F24" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG15n.jpg</v>
+        <v>MA_07_05_REC10_IMG15n.jpg</v>
       </c>
       <c r="G24" s="13" t="str">
         <f ca="1">IF($F24&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E24,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -4005,17 +4005,17 @@
       </c>
       <c r="H24" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG15a.jpg</v>
+        <v>MA_07_05_REC10_IMG15a.jpg</v>
       </c>
       <c r="I24" s="13" t="str">
         <f ca="1">IF(OR($B24&lt;&gt;"",$J24&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E24,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E24,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J24" s="63" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K24" s="64" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O24" s="2" t="str">
         <f>'Definición técnica de imagenes'!A37</f>
@@ -4028,7 +4028,7 @@
         <v>IMG16</v>
       </c>
       <c r="B25" s="62" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C25" s="20" t="str">
         <f t="shared" si="0"/>
@@ -4042,7 +4042,7 @@
       </c>
       <c r="F25" s="13" t="str">
         <f t="shared" ca="1" si="4"/>
-        <v>MA_09_02_REC10_IMG16n.jpg</v>
+        <v>MA_07_05_REC10_IMG16n.jpg</v>
       </c>
       <c r="G25" s="13" t="str">
         <f ca="1">IF($F25&lt;&gt;"",IF($G$4="Recurso",VLOOKUP($E25,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),5),5,FALSE),'Definición técnica de imagenes'!$F$16),"")</f>
@@ -4050,17 +4050,17 @@
       </c>
       <c r="H25" s="13" t="str">
         <f t="shared" ca="1" si="5"/>
-        <v>MA_09_02_REC10_IMG16a.jpg</v>
+        <v>MA_07_05_REC10_IMG16a.jpg</v>
       </c>
       <c r="I25" s="13" t="str">
         <f ca="1">IF(OR($B25&lt;&gt;"",$J25&lt;&gt;""),IF($G$4="Recurso",IF(VLOOKUP($E25,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)=0,"",VLOOKUP($E25,OFFSET('Definición técnica de imagenes'!$A$1,MATCH($G$5,'Definición técnica de imagenes'!$A$1:$A$104,0)-1,1,COUNTIF('Definición técnica de imagenes'!$A$3:$A$102,$G$5),6),6,FALSE)),'Definición técnica de imagenes'!$G$16),"")</f>
         <v>800 x 458 px</v>
       </c>
       <c r="J25" s="63" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K25" s="64" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
@@ -6707,25 +6707,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="85" t="s">
+      <c r="A1" s="87" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="87"/>
+      <c r="B1" s="88"/>
+      <c r="C1" s="88"/>
+      <c r="D1" s="88"/>
+      <c r="E1" s="88"/>
+      <c r="F1" s="89"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="30" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="31"/>
-      <c r="C2" s="88" t="s">
+      <c r="C2" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="90"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="92"/>
       <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:11" ht="62" x14ac:dyDescent="0.35">
@@ -6733,11 +6733,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="31"/>
-      <c r="C3" s="94" t="s">
+      <c r="C3" s="96" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="95"/>
-      <c r="E3" s="96"/>
+      <c r="D3" s="97"/>
+      <c r="E3" s="98"/>
       <c r="F3" s="32"/>
       <c r="H3" s="22" t="s">
         <v>18</v>
@@ -6788,11 +6788,11 @@
       <c r="C5" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="97" t="str">
+      <c r="D5" s="99" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="98"/>
+      <c r="E5" s="100"/>
       <c r="F5" s="32"/>
       <c r="H5" s="22" t="s">
         <v>22</v>
@@ -6837,12 +6837,12 @@
       <c r="C7" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="83" t="str">
+      <c r="D7" s="85" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="83"/>
-      <c r="F7" s="84"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="86"/>
       <c r="H7" s="22" t="s">
         <v>24</v>
       </c>
@@ -6936,14 +6936,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="85" t="s">
+      <c r="A13" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="86"/>
-      <c r="C13" s="86"/>
-      <c r="D13" s="86"/>
-      <c r="E13" s="86"/>
-      <c r="F13" s="87"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="88"/>
+      <c r="F13" s="89"/>
       <c r="I13" s="22" t="s">
         <v>33</v>
       </c>
@@ -6976,12 +6976,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="31"/>
-      <c r="C15" s="88" t="s">
+      <c r="C15" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="90"/>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="92"/>
       <c r="J15" s="22">
         <v>12</v>
       </c>
@@ -7021,12 +7021,12 @@
       <c r="C17" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="91" t="str">
+      <c r="D17" s="93" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="92"/>
-      <c r="F17" s="93"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="95"/>
       <c r="J17" s="22">
         <v>14</v>
       </c>
@@ -7042,12 +7042,12 @@
       <c r="C18" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="83" t="str">
+      <c r="D18" s="85" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="83"/>
-      <c r="F18" s="84"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="86"/>
       <c r="J18" s="22">
         <v>15</v>
       </c>
@@ -7438,40 +7438,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="102" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="100" t="s">
+      <c r="B1" s="102" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="100" t="s">
+      <c r="C1" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="100" t="s">
+      <c r="D1" s="102" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="100" t="s">
+      <c r="E1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="100" t="s">
+      <c r="F1" s="102" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="100" t="s">
+      <c r="G1" s="102" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="99" t="s">
+      <c r="H1" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="99"/>
+      <c r="I1" s="101"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="100"/>
-      <c r="B2" s="100"/>
-      <c r="C2" s="100"/>
-      <c r="D2" s="100"/>
-      <c r="E2" s="100"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
+      <c r="A2" s="102"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
       <c r="H2" s="39" t="s">
         <v>65</v>
       </c>

</xml_diff>